<commit_message>
update weights and render
</commit_message>
<xml_diff>
--- a/kattungar.xlsx
+++ b/kattungar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\git\cats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A12560-0EB0-408A-B98C-DAAF21BADFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50598DC1-6E6E-4565-8B7D-F9F367B96DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{36296AD2-3383-4412-B526-17245D0827CA}"/>
   </bookViews>
@@ -335,9 +335,9 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Blad1!$G$2:$G$41</c:f>
+              <c:f>Blad1!$G$2:$G$46</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>45388,46</c:v>
                 </c:pt>
@@ -453,6 +453,21 @@
                   <c:v>45411,42</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>45414,31</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45415,42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45416,42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45416,83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45417,44</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v> </c:v>
                 </c:pt>
               </c:strCache>
@@ -460,10 +475,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$H$2:$H$41</c:f>
+              <c:f>Blad1!$H$2:$H$46</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -577,6 +592,21 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>1.8285714285714287</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.0914285714285716</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.1085714285714285</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.137142857142857</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.1714285714285713</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.2685714285714287</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -634,9 +664,9 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Blad1!$G$2:$G$41</c:f>
+              <c:f>Blad1!$G$2:$G$46</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>45388,46</c:v>
                 </c:pt>
@@ -752,6 +782,21 @@
                   <c:v>45411,42</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>45414,31</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45415,42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45416,42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45416,83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45417,44</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v> </c:v>
                 </c:pt>
               </c:strCache>
@@ -759,10 +804,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$I$2:$I$41</c:f>
+              <c:f>Blad1!$I$2:$I$46</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -876,6 +921,21 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>1.8975903614457832</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.1024096385542168</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.1686746987951806</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.1506024096385543</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.1927710843373496</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.3132530120481927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -931,9 +991,9 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Blad1!$G$2:$G$41</c:f>
+              <c:f>Blad1!$G$2:$G$46</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>45388,46</c:v>
                 </c:pt>
@@ -1049,6 +1109,21 @@
                   <c:v>45411,42</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>45414,31</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45415,42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45416,42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45416,83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45417,44</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v> </c:v>
                 </c:pt>
               </c:strCache>
@@ -1056,10 +1131,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$J$2:$J$41</c:f>
+              <c:f>Blad1!$J$2:$J$46</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1173,6 +1248,21 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>3.0740740740740744</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.4629629629629628</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.4444444444444446</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.5185185185185182</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.6296296296296298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1224,9 +1314,9 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Blad1!$G$2:$G$41</c:f>
+              <c:f>Blad1!$G$2:$G$46</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>45388,46</c:v>
                 </c:pt>
@@ -1342,6 +1432,21 @@
                   <c:v>45411,42</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>45414,31</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45415,42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45416,42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45416,83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45417,44</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v> </c:v>
                 </c:pt>
               </c:strCache>
@@ -1349,10 +1454,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$K$2:$K$41</c:f>
+              <c:f>Blad1!$K$2:$K$46</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1466,6 +1571,21 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>2.2546583850931676</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.4472049689440993</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.5031055900621118</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.5217391304347827</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.652173913043478</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.7391304347826089</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1791,9 +1911,9 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Blad1!$G$2:$G$41</c:f>
+              <c:f>Blad1!$G$2:$G$46</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>45388,46</c:v>
                 </c:pt>
@@ -1909,6 +2029,21 @@
                   <c:v>45411,42</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>45414,31</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45415,42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45416,42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45416,83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45417,44</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v> </c:v>
                 </c:pt>
               </c:strCache>
@@ -1916,10 +2051,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$B$2:$B$41</c:f>
+              <c:f>Blad1!$B$2:$B$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>175</c:v>
                 </c:pt>
@@ -2033,6 +2168,21 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>541</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>549</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>572</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2090,9 +2240,9 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Blad1!$G$2:$G$41</c:f>
+              <c:f>Blad1!$G$2:$G$46</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>45388,46</c:v>
                 </c:pt>
@@ -2208,6 +2358,21 @@
                   <c:v>45411,42</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>45414,31</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45415,42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45416,42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45416,83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45417,44</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v> </c:v>
                 </c:pt>
               </c:strCache>
@@ -2215,10 +2380,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$C$2:$C$41</c:f>
+              <c:f>Blad1!$C$2:$C$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>166</c:v>
                 </c:pt>
@@ -2332,6 +2497,21 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>481</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>523</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>550</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2387,9 +2567,9 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Blad1!$G$2:$G$41</c:f>
+              <c:f>Blad1!$G$2:$G$46</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>45388,46</c:v>
                 </c:pt>
@@ -2505,6 +2685,21 @@
                   <c:v>45411,42</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>45414,31</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45415,42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45416,42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45416,83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45417,44</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v> </c:v>
                 </c:pt>
               </c:strCache>
@@ -2512,10 +2707,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$D$2:$D$41</c:f>
+              <c:f>Blad1!$D$2:$D$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>108</c:v>
                 </c:pt>
@@ -2629,6 +2824,21 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>482</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>488</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2680,9 +2890,9 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Blad1!$G$2:$G$41</c:f>
+              <c:f>Blad1!$G$2:$G$46</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>45388,46</c:v>
                 </c:pt>
@@ -2798,6 +3008,21 @@
                   <c:v>45411,42</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>45414,31</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45415,42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45416,42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45416,83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45417,44</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v> </c:v>
                 </c:pt>
               </c:strCache>
@@ -2805,10 +3030,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$E$2:$E$41</c:f>
+              <c:f>Blad1!$E$2:$E$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>161</c:v>
                 </c:pt>
@@ -2922,6 +3147,21 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>524</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>564</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>567</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>588</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>602</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3249,9 +3489,9 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Blad1!$G$2:$G$41</c:f>
+              <c:f>Blad1!$G$2:$G$46</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>45388,46</c:v>
                 </c:pt>
@@ -3367,6 +3607,21 @@
                   <c:v>45411,42</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>45414,31</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45415,42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45416,42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45416,83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45417,44</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v> </c:v>
                 </c:pt>
               </c:strCache>
@@ -3374,10 +3629,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$P$2:$P$41</c:f>
+              <c:f>Blad1!$P$2:$P$46</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3491,6 +3746,21 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>14.181818181855704</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>15.884892086317631</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.7169812744693629</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14.399997999994362</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>28.137931034595713</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3546,9 +3816,9 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Blad1!$G$2:$G$41</c:f>
+              <c:f>Blad1!$G$2:$G$46</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>45388,46</c:v>
                 </c:pt>
@@ -3664,6 +3934,21 @@
                   <c:v>45411,42</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>45414,31</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45415,42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45416,42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45416,83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45417,44</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v> </c:v>
                 </c:pt>
               </c:strCache>
@@ -3671,10 +3956,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$Q$2:$Q$41</c:f>
+              <c:f>Blad1!$Q$2:$Q$46</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3788,6 +4073,21 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>4.3636363636479087</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11.74100719423477</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.9622646730543298</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>16.79999766666009</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>33.103448275994957</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3843,9 +4143,9 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Blad1!$G$2:$G$41</c:f>
+              <c:f>Blad1!$G$2:$G$46</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>45388,46</c:v>
                 </c:pt>
@@ -3961,6 +4261,21 @@
                   <c:v>45411,42</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>45414,31</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45415,42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45416,42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45416,83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45417,44</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v> </c:v>
                 </c:pt>
               </c:strCache>
@@ -3968,10 +4283,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$R$2:$R$41</c:f>
+              <c:f>Blad1!$R$2:$R$46</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4085,6 +4400,21 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>24.000000000063498</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.6690647481933407</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>12.679245947523693</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>19.199997333325815</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>19.862068965596976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4136,9 +4466,9 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Blad1!$G$2:$G$41</c:f>
+              <c:f>Blad1!$G$2:$G$46</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>45388,46</c:v>
                 </c:pt>
@@ -4254,6 +4584,21 @@
                   <c:v>45411,42</c:v>
                 </c:pt>
                 <c:pt idx="38">
+                  <c:v>45414,31</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45415,42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45416,42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45416,83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45417,44</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v> </c:v>
                 </c:pt>
               </c:strCache>
@@ -4261,10 +4606,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Blad1!$S$2:$S$41</c:f>
+              <c:f>Blad1!$S$2:$S$46</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="40"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4378,6 +4723,21 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>29.454545454623386</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10.705035971214055</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.1509438234080882</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>50.39999299998027</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>23.172413793196469</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6278,13 +6638,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6316,13 +6676,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6354,13 +6714,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6708,11 +7068,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33456F3-4980-430D-BFBA-60DE0169B3D8}">
-  <dimension ref="A1:T42"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P33" sqref="P33:S39"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H36" sqref="H36:S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6871,7 +7231,7 @@
         <v>167</v>
       </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G3:G39" si="2">A3</f>
+        <f t="shared" ref="G3:G44" si="2">A3</f>
         <v>45388.607638888891</v>
       </c>
       <c r="H3" s="13">
@@ -8133,35 +8493,35 @@
         <v>45397.375</v>
       </c>
       <c r="H21" s="13">
-        <f t="shared" ref="H21:H39" si="31">B21/B$2-1</f>
+        <f t="shared" ref="H21:H44" si="31">B21/B$2-1</f>
         <v>0.68571428571428572</v>
       </c>
       <c r="I21" s="13">
-        <f t="shared" ref="I21:I39" si="32">C21/C$2-1</f>
+        <f t="shared" ref="I21:I43" si="32">C21/C$2-1</f>
         <v>0.72289156626506035</v>
       </c>
       <c r="J21" s="13">
-        <f t="shared" ref="J21:J39" si="33">D21/D$2-1</f>
+        <f t="shared" ref="J21:J44" si="33">D21/D$2-1</f>
         <v>1.2129629629629628</v>
       </c>
       <c r="K21" s="13">
-        <f t="shared" ref="K21:K39" si="34">E21/E$2-1</f>
+        <f t="shared" ref="K21:K44" si="34">E21/E$2-1</f>
         <v>0.75155279503105588</v>
       </c>
       <c r="L21" s="20">
-        <f t="shared" ref="L21:L39" si="35">B21-B$2</f>
+        <f t="shared" ref="L21:L44" si="35">B21-B$2</f>
         <v>120</v>
       </c>
       <c r="M21" s="20">
-        <f t="shared" ref="M21:M39" si="36">C21-C$2</f>
+        <f t="shared" ref="M21:M43" si="36">C21-C$2</f>
         <v>120</v>
       </c>
       <c r="N21" s="20">
-        <f t="shared" ref="N21:N39" si="37">E21-D$2</f>
+        <f t="shared" ref="N21:N44" si="37">E21-D$2</f>
         <v>174</v>
       </c>
       <c r="O21" s="20">
-        <f t="shared" ref="O21:O39" si="38">E21-E$2</f>
+        <f t="shared" ref="O21:O44" si="38">E21-E$2</f>
         <v>121</v>
       </c>
       <c r="P21" s="21">
@@ -9237,51 +9597,51 @@
         <v>45409.916666666664</v>
       </c>
       <c r="H37" s="13">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="H37:H44" si="55">B37/B$2-1</f>
         <v>1.7771428571428571</v>
       </c>
       <c r="I37" s="13">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="I37:I44" si="56">C37/C$2-1</f>
         <v>1.7771084337349397</v>
       </c>
       <c r="J37" s="13">
-        <f t="shared" si="33"/>
+        <f t="shared" ref="J37:J44" si="57">D37/D$2-1</f>
         <v>2.7685185185185186</v>
       </c>
       <c r="K37" s="13">
-        <f t="shared" si="34"/>
+        <f t="shared" ref="K37:K44" si="58">E37/E$2-1</f>
         <v>2.012422360248447</v>
       </c>
       <c r="L37" s="20">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="L37:L44" si="59">B37-B$2</f>
         <v>311</v>
       </c>
       <c r="M37" s="20">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="M37:M44" si="60">C37-C$2</f>
         <v>295</v>
       </c>
       <c r="N37" s="20">
-        <f t="shared" si="37"/>
+        <f t="shared" ref="N37:N44" si="61">E37-D$2</f>
         <v>377</v>
       </c>
       <c r="O37" s="20">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="O37:O44" si="62">E37-E$2</f>
         <v>324</v>
       </c>
       <c r="P37" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" ref="P37:P44" si="63">(B37-B36)/(G37-G36)</f>
         <v>21.230769230864293</v>
       </c>
       <c r="Q37" s="21">
-        <f t="shared" si="52"/>
+        <f t="shared" ref="Q37:Q44" si="64">(C37-C36)/($G37-$G36)</f>
         <v>7.3846153846484492</v>
       </c>
       <c r="R37" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="R37:R44" si="65">(D37-D36)/($G37-$G36)</f>
         <v>8.3076923077295053</v>
       </c>
       <c r="S37" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" ref="S37:S44" si="66">(E37-E36)/($G37-$G36)</f>
         <v>-1.8461538461621123</v>
       </c>
     </row>
@@ -9306,51 +9666,51 @@
         <v>45410.5</v>
       </c>
       <c r="H38" s="13">
-        <f t="shared" si="31"/>
+        <f t="shared" si="55"/>
         <v>1.7542857142857144</v>
       </c>
       <c r="I38" s="13">
-        <f t="shared" si="32"/>
+        <f t="shared" si="56"/>
         <v>1.8734939759036147</v>
       </c>
       <c r="J38" s="13">
-        <f t="shared" si="33"/>
+        <f t="shared" si="57"/>
         <v>2.8703703703703702</v>
       </c>
       <c r="K38" s="13">
-        <f t="shared" si="34"/>
+        <f t="shared" si="58"/>
         <v>2.0869565217391304</v>
       </c>
       <c r="L38" s="20">
-        <f t="shared" si="35"/>
+        <f t="shared" si="59"/>
         <v>307</v>
       </c>
       <c r="M38" s="20">
-        <f t="shared" si="36"/>
+        <f t="shared" si="60"/>
         <v>311</v>
       </c>
       <c r="N38" s="20">
-        <f t="shared" si="37"/>
+        <f t="shared" si="61"/>
         <v>389</v>
       </c>
       <c r="O38" s="20">
-        <f t="shared" si="38"/>
+        <f t="shared" si="62"/>
         <v>336</v>
       </c>
       <c r="P38" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>-6.8571428571143471</v>
       </c>
       <c r="Q38" s="21">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>27.428571428457388</v>
       </c>
       <c r="R38" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="65"/>
         <v>18.857142857064456</v>
       </c>
       <c r="S38" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="66"/>
         <v>20.571428571343041</v>
       </c>
     </row>
@@ -9375,85 +9735,433 @@
         <v>45411.416666666664</v>
       </c>
       <c r="H39" s="13">
-        <f t="shared" si="31"/>
+        <f t="shared" si="55"/>
         <v>1.8285714285714287</v>
       </c>
       <c r="I39" s="13">
-        <f t="shared" si="32"/>
+        <f t="shared" si="56"/>
         <v>1.8975903614457832</v>
       </c>
       <c r="J39" s="13">
-        <f t="shared" si="33"/>
+        <f t="shared" si="57"/>
         <v>3.0740740740740744</v>
       </c>
       <c r="K39" s="13">
-        <f t="shared" si="34"/>
+        <f t="shared" si="58"/>
         <v>2.2546583850931676</v>
       </c>
       <c r="L39" s="20">
-        <f t="shared" si="35"/>
+        <f t="shared" si="59"/>
         <v>320</v>
       </c>
       <c r="M39" s="20">
-        <f t="shared" si="36"/>
+        <f t="shared" si="60"/>
         <v>315</v>
       </c>
       <c r="N39" s="20">
-        <f t="shared" si="37"/>
+        <f t="shared" si="61"/>
         <v>416</v>
       </c>
       <c r="O39" s="20">
-        <f t="shared" si="38"/>
+        <f t="shared" si="62"/>
         <v>363</v>
       </c>
       <c r="P39" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>14.181818181855704</v>
       </c>
       <c r="Q39" s="21">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>4.3636363636479087</v>
       </c>
       <c r="R39" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="65"/>
         <v>24.000000000063498</v>
       </c>
       <c r="S39" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="66"/>
         <v>29.454545454623386</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G40" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-      <c r="O40" s="20"/>
-      <c r="P40" s="21"/>
-      <c r="Q40" s="21"/>
-      <c r="R40" s="21"/>
-      <c r="S40" s="21"/>
+      <c r="A40" s="1">
+        <v>45414.3125</v>
+      </c>
+      <c r="B40" s="4">
+        <v>541</v>
+      </c>
+      <c r="C40" s="4">
+        <v>515</v>
+      </c>
+      <c r="D40" s="4">
+        <v>468</v>
+      </c>
+      <c r="E40" s="4">
+        <v>555</v>
+      </c>
+      <c r="G40" s="3">
+        <f t="shared" si="2"/>
+        <v>45414.3125</v>
+      </c>
+      <c r="H40" s="13">
+        <f t="shared" si="55"/>
+        <v>2.0914285714285716</v>
+      </c>
+      <c r="I40" s="13">
+        <f t="shared" si="56"/>
+        <v>2.1024096385542168</v>
+      </c>
+      <c r="J40" s="13">
+        <f t="shared" si="57"/>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="K40" s="13">
+        <f t="shared" si="58"/>
+        <v>2.4472049689440993</v>
+      </c>
+      <c r="L40" s="20">
+        <f t="shared" si="59"/>
+        <v>366</v>
+      </c>
+      <c r="M40" s="20">
+        <f t="shared" si="60"/>
+        <v>349</v>
+      </c>
+      <c r="N40" s="20">
+        <f t="shared" si="61"/>
+        <v>447</v>
+      </c>
+      <c r="O40" s="20">
+        <f t="shared" si="62"/>
+        <v>394</v>
+      </c>
+      <c r="P40" s="21">
+        <f t="shared" si="63"/>
+        <v>15.884892086317631</v>
+      </c>
+      <c r="Q40" s="21">
+        <f t="shared" si="64"/>
+        <v>11.74100719423477</v>
+      </c>
+      <c r="R40" s="21">
+        <f t="shared" si="65"/>
+        <v>9.6690647481933407</v>
+      </c>
+      <c r="S40" s="21">
+        <f t="shared" si="66"/>
+        <v>10.705035971214055</v>
+      </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="P41" s="21"/>
-      <c r="Q41" s="21"/>
-      <c r="R41" s="21"/>
-      <c r="S41" s="21"/>
+      <c r="A41" s="1">
+        <v>45415.416666608799</v>
+      </c>
+      <c r="B41" s="4">
+        <v>544</v>
+      </c>
+      <c r="C41" s="4">
+        <v>526</v>
+      </c>
+      <c r="D41" s="4">
+        <v>482</v>
+      </c>
+      <c r="E41" s="4">
+        <v>564</v>
+      </c>
+      <c r="G41" s="3">
+        <f t="shared" si="2"/>
+        <v>45415.416666608799</v>
+      </c>
+      <c r="H41" s="13">
+        <f t="shared" si="55"/>
+        <v>2.1085714285714285</v>
+      </c>
+      <c r="I41" s="13">
+        <f t="shared" si="56"/>
+        <v>2.1686746987951806</v>
+      </c>
+      <c r="J41" s="13">
+        <f t="shared" si="57"/>
+        <v>3.4629629629629628</v>
+      </c>
+      <c r="K41" s="13">
+        <f t="shared" si="58"/>
+        <v>2.5031055900621118</v>
+      </c>
+      <c r="L41" s="20">
+        <f t="shared" si="59"/>
+        <v>369</v>
+      </c>
+      <c r="M41" s="20">
+        <f t="shared" si="60"/>
+        <v>360</v>
+      </c>
+      <c r="N41" s="20">
+        <f t="shared" si="61"/>
+        <v>456</v>
+      </c>
+      <c r="O41" s="20">
+        <f t="shared" si="62"/>
+        <v>403</v>
+      </c>
+      <c r="P41" s="21">
+        <f t="shared" si="63"/>
+        <v>2.7169812744693629</v>
+      </c>
+      <c r="Q41" s="21">
+        <f t="shared" si="64"/>
+        <v>9.9622646730543298</v>
+      </c>
+      <c r="R41" s="21">
+        <f t="shared" si="65"/>
+        <v>12.679245947523693</v>
+      </c>
+      <c r="S41" s="21">
+        <f t="shared" si="66"/>
+        <v>8.1509438234080882</v>
+      </c>
     </row>
-    <row r="42" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="18"/>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>45416.416666608799</v>
+      </c>
+      <c r="B42" s="4">
+        <v>549</v>
+      </c>
+      <c r="C42" s="4">
+        <v>523</v>
+      </c>
+      <c r="D42" s="4">
+        <v>480</v>
+      </c>
+      <c r="E42" s="4">
+        <v>567</v>
+      </c>
+      <c r="G42" s="3">
+        <f t="shared" si="2"/>
+        <v>45416.416666608799</v>
+      </c>
+      <c r="H42" s="13">
+        <f t="shared" si="55"/>
+        <v>2.137142857142857</v>
+      </c>
+      <c r="I42" s="13">
+        <f t="shared" si="56"/>
+        <v>2.1506024096385543</v>
+      </c>
+      <c r="J42" s="13">
+        <f t="shared" si="57"/>
+        <v>3.4444444444444446</v>
+      </c>
+      <c r="K42" s="13">
+        <f t="shared" si="58"/>
+        <v>2.5217391304347827</v>
+      </c>
+      <c r="L42" s="20">
+        <f t="shared" si="59"/>
+        <v>374</v>
+      </c>
+      <c r="M42" s="20">
+        <f t="shared" si="60"/>
+        <v>357</v>
+      </c>
+      <c r="N42" s="20">
+        <f t="shared" si="61"/>
+        <v>459</v>
+      </c>
+      <c r="O42" s="20">
+        <f t="shared" si="62"/>
+        <v>406</v>
+      </c>
+      <c r="P42" s="21">
+        <f t="shared" si="63"/>
+        <v>5</v>
+      </c>
+      <c r="Q42" s="21">
+        <f t="shared" si="64"/>
+        <v>-3</v>
+      </c>
+      <c r="R42" s="21">
+        <f t="shared" si="65"/>
+        <v>-2</v>
+      </c>
+      <c r="S42" s="21">
+        <f t="shared" si="66"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>45416.833333333336</v>
+      </c>
+      <c r="B43" s="4">
+        <v>555</v>
+      </c>
+      <c r="C43" s="4">
+        <v>530</v>
+      </c>
+      <c r="D43" s="4">
+        <v>488</v>
+      </c>
+      <c r="E43" s="4">
+        <v>588</v>
+      </c>
+      <c r="G43" s="3">
+        <f t="shared" si="2"/>
+        <v>45416.833333333336</v>
+      </c>
+      <c r="H43" s="13">
+        <f t="shared" si="55"/>
+        <v>2.1714285714285713</v>
+      </c>
+      <c r="I43" s="13">
+        <f t="shared" si="56"/>
+        <v>2.1927710843373496</v>
+      </c>
+      <c r="J43" s="13">
+        <f t="shared" si="57"/>
+        <v>3.5185185185185182</v>
+      </c>
+      <c r="K43" s="13">
+        <f t="shared" si="58"/>
+        <v>2.652173913043478</v>
+      </c>
+      <c r="L43" s="20">
+        <f t="shared" si="59"/>
+        <v>380</v>
+      </c>
+      <c r="M43" s="20">
+        <f t="shared" si="60"/>
+        <v>364</v>
+      </c>
+      <c r="N43" s="20">
+        <f t="shared" si="61"/>
+        <v>480</v>
+      </c>
+      <c r="O43" s="20">
+        <f t="shared" si="62"/>
+        <v>427</v>
+      </c>
+      <c r="P43" s="21">
+        <f t="shared" si="63"/>
+        <v>14.399997999994362</v>
+      </c>
+      <c r="Q43" s="21">
+        <f t="shared" si="64"/>
+        <v>16.79999766666009</v>
+      </c>
+      <c r="R43" s="21">
+        <f t="shared" si="65"/>
+        <v>19.199997333325815</v>
+      </c>
+      <c r="S43" s="21">
+        <f t="shared" si="66"/>
+        <v>50.39999299998027</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>45417.4375</v>
+      </c>
+      <c r="B44" s="4">
+        <v>572</v>
+      </c>
+      <c r="C44" s="4">
+        <v>550</v>
+      </c>
+      <c r="D44" s="4">
+        <v>500</v>
+      </c>
+      <c r="E44" s="4">
+        <v>602</v>
+      </c>
+      <c r="G44" s="3">
+        <f t="shared" si="2"/>
+        <v>45417.4375</v>
+      </c>
+      <c r="H44" s="13">
+        <f t="shared" si="55"/>
+        <v>2.2685714285714287</v>
+      </c>
+      <c r="I44" s="13">
+        <f t="shared" si="56"/>
+        <v>2.3132530120481927</v>
+      </c>
+      <c r="J44" s="13">
+        <f t="shared" si="57"/>
+        <v>3.6296296296296298</v>
+      </c>
+      <c r="K44" s="13">
+        <f t="shared" si="58"/>
+        <v>2.7391304347826089</v>
+      </c>
+      <c r="L44" s="20">
+        <f t="shared" si="59"/>
+        <v>397</v>
+      </c>
+      <c r="M44" s="20">
+        <f t="shared" si="60"/>
+        <v>384</v>
+      </c>
+      <c r="N44" s="20">
+        <f t="shared" si="61"/>
+        <v>494</v>
+      </c>
+      <c r="O44" s="20">
+        <f t="shared" si="62"/>
+        <v>441</v>
+      </c>
+      <c r="P44" s="21">
+        <f t="shared" si="63"/>
+        <v>28.137931034595713</v>
+      </c>
+      <c r="Q44" s="21">
+        <f t="shared" si="64"/>
+        <v>33.103448275994957</v>
+      </c>
+      <c r="R44" s="21">
+        <f t="shared" si="65"/>
+        <v>19.862068965596976</v>
+      </c>
+      <c r="S44" s="21">
+        <f t="shared" si="66"/>
+        <v>23.172413793196469</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>45418.416666608799</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="20"/>
+      <c r="O45" s="20"/>
+      <c r="P45" s="21"/>
+      <c r="Q45" s="21"/>
+      <c r="R45" s="21"/>
+      <c r="S45" s="21"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P46" s="21"/>
+      <c r="Q46" s="21"/>
+      <c r="R46" s="21"/>
+      <c r="S46" s="21"/>
+    </row>
+    <row r="47" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>